<commit_message>
Swapping this to be my main repo
</commit_message>
<xml_diff>
--- a/working_data/function_1_data.xlsx
+++ b/working_data/function_1_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="6">
   <si>
     <t>X_1</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -927,6 +927,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>0.596596</v>
+      </c>
+      <c r="B39">
+        <v>0.644644</v>
+      </c>
+      <c r="C39">
+        <v>0.05961267486908179</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>0.596596</v>
+      </c>
+      <c r="B40">
+        <v>0.627627</v>
+      </c>
+      <c r="C40">
+        <v>0.1126700295757865</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new predictions. Added meshgrid & localize()
</commit_message>
<xml_diff>
--- a/working_data/function_1_data.xlsx
+++ b/working_data/function_1_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="6">
   <si>
     <t>X_1</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -955,6 +955,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>0.568568</v>
+      </c>
+      <c r="B41">
+        <v>0.627627</v>
+      </c>
+      <c r="C41">
+        <v>-0.004658275856841883</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>